<commit_message>
PMP 수정, 1024 백지수 PSP 수정, UC Spec 수정
</commit_message>
<xml_diff>
--- a/Project Planning/1_3_PSP_Sheet.xlsx
+++ b/Project Planning/1_3_PSP_Sheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\최재영\Desktop\babalzza-master\Project Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Desktop\babalzza-master\babalzza-master\Project Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26835" windowHeight="12015" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26832" windowHeight="12012"/>
   </bookViews>
   <sheets>
     <sheet name="백지수" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="황보진우" sheetId="6" r:id="rId6"/>
     <sheet name="팀 통합" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1299,7 +1299,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="128">
   <si>
     <r>
       <rPr>
@@ -6001,6 +6001,404 @@
         <family val="2"/>
       </rPr>
       <t>)</t>
+    </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>10</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 23</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Software Requirement Spectification 1.0</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Initial Data Set </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>제작</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>준비</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>메뉴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>엑셀</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>채워넣기</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>기타</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 24</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Initial Data Set </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>제작</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>준비</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>설문조사</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>폼</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>제작</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>메뉴추천</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 24</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일</t>
+    </r>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">UC Diagram + UC Spec </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>수정</t>
     </r>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
@@ -6008,7 +6406,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="176" formatCode="m&quot;월&quot;\ d&quot;일&quot;;@"/>
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
@@ -6162,7 +6560,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -6302,6 +6700,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="백분율" xfId="1" builtinId="5"/>
@@ -6618,21 +7017,21 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="46.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="46.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
@@ -6645,10 +7044,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
     </row>
-    <row r="3" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>39</v>
       </c>
@@ -6659,8 +7058,8 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:7" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:7" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>32</v>
       </c>
@@ -6683,7 +7082,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
@@ -6706,7 +7105,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>43</v>
       </c>
@@ -6729,7 +7128,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>44</v>
       </c>
@@ -6752,7 +7151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>54</v>
       </c>
@@ -6775,7 +7174,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>52</v>
       </c>
@@ -6798,7 +7197,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>55</v>
       </c>
@@ -6821,7 +7220,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>55</v>
       </c>
@@ -6844,7 +7243,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>42</v>
       </c>
@@ -6867,7 +7266,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>42</v>
       </c>
@@ -6890,7 +7289,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>49</v>
       </c>
@@ -6913,7 +7312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>50</v>
       </c>
@@ -6936,7 +7335,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>45</v>
       </c>
@@ -6959,7 +7358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>47</v>
       </c>
@@ -6982,7 +7381,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>53</v>
       </c>
@@ -7005,7 +7404,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="43" t="s">
         <v>46</v>
       </c>
@@ -7028,7 +7427,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
         <v>48</v>
       </c>
@@ -7051,7 +7450,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="43" t="s">
         <v>51</v>
       </c>
@@ -7074,7 +7473,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="53" t="s">
         <v>84</v>
       </c>
@@ -7097,7 +7496,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="53" t="s">
         <v>87</v>
       </c>
@@ -7120,7 +7519,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A25" s="53" t="s">
         <v>90</v>
       </c>
@@ -7143,34 +7542,76 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="4"/>
-    </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A26" s="73" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="17">
+        <v>60</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="G26" s="72" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="73" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="17">
+        <v>120</v>
+      </c>
+      <c r="F27" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="G27" s="72" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C28" s="3">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="D28" s="9">
+        <v>10</v>
+      </c>
+      <c r="E28" s="17">
+        <v>60</v>
+      </c>
+      <c r="F28" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="G28" s="72" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -7179,7 +7620,7 @@
       <c r="F29" s="17"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -7188,7 +7629,7 @@
       <c r="F30" s="17"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -7197,7 +7638,7 @@
       <c r="F31" s="17"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -7206,7 +7647,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -7215,7 +7656,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -7224,7 +7665,7 @@
       <c r="F34" s="17"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -7233,7 +7674,7 @@
       <c r="F35" s="17"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -7242,7 +7683,7 @@
       <c r="F36" s="9"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -7251,7 +7692,7 @@
       <c r="F37" s="9"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -7263,11 +7704,11 @@
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"돋움,Regular"&amp;8Adapted from &amp;"돋움,Italic"A Discipline for Software Engineering,&amp;"돋움,Regular"by Watts Humphrey. Addison-Wesley Publishing Company, 1995</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7280,17 +7721,17 @@
       <selection activeCell="A12" sqref="A12:G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="55.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="25.5546875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="55.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
@@ -7303,10 +7744,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
     </row>
-    <row r="3" spans="1:10" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>39</v>
       </c>
@@ -7317,8 +7758,8 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:10" ht="11.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:10" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:10" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>32</v>
       </c>
@@ -7341,7 +7782,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>44</v>
       </c>
@@ -7364,7 +7805,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>55</v>
       </c>
@@ -7387,7 +7828,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>55</v>
       </c>
@@ -7410,7 +7851,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>42</v>
       </c>
@@ -7433,7 +7874,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -7456,7 +7897,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>45</v>
       </c>
@@ -7479,7 +7920,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="39" t="s">
         <v>29</v>
       </c>
@@ -7503,7 +7944,7 @@
       </c>
       <c r="J12" s="22"/>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="39" t="s">
         <v>37</v>
       </c>
@@ -7526,7 +7967,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A14" s="39" t="s">
         <v>33</v>
       </c>
@@ -7549,7 +7990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -7558,7 +7999,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -7567,7 +8008,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -7576,7 +8017,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -7585,7 +8026,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="19"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -7594,7 +8035,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -7603,7 +8044,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -7612,7 +8053,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -7621,7 +8062,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -7630,7 +8071,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -7639,7 +8080,7 @@
       <c r="F24" s="17"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -7648,7 +8089,7 @@
       <c r="F25" s="17"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -7657,7 +8098,7 @@
       <c r="F26" s="17"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -7666,7 +8107,7 @@
       <c r="F27" s="17"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -7675,7 +8116,7 @@
       <c r="F28" s="17"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -7684,7 +8125,7 @@
       <c r="F29" s="17"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -7693,7 +8134,7 @@
       <c r="F30" s="17"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -7702,7 +8143,7 @@
       <c r="F31" s="17"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -7711,7 +8152,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -7720,7 +8161,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -7729,7 +8170,7 @@
       <c r="F34" s="17"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -7738,7 +8179,7 @@
       <c r="F35" s="17"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -7747,7 +8188,7 @@
       <c r="F36" s="9"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -7756,7 +8197,7 @@
       <c r="F37" s="9"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -7785,17 +8226,17 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="61.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="61.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
@@ -7808,10 +8249,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
     </row>
-    <row r="3" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>39</v>
       </c>
@@ -7822,8 +8263,8 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:7" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:7" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>32</v>
       </c>
@@ -7846,7 +8287,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>43715</v>
       </c>
@@ -7869,7 +8310,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>43727</v>
       </c>
@@ -7892,7 +8333,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>43727</v>
       </c>
@@ -7915,7 +8356,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>43728</v>
       </c>
@@ -7938,7 +8379,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27">
         <v>43735</v>
       </c>
@@ -7961,7 +8402,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31">
         <v>43736</v>
       </c>
@@ -7984,7 +8425,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="27">
         <v>43737</v>
       </c>
@@ -8007,7 +8448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>43739</v>
       </c>
@@ -8030,7 +8471,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="59">
         <v>43739</v>
       </c>
@@ -8053,7 +8494,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="59">
         <v>43743</v>
       </c>
@@ -8076,7 +8517,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="59">
         <v>43744</v>
       </c>
@@ -8099,7 +8540,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="59">
         <v>43745</v>
       </c>
@@ -8122,7 +8563,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="59">
         <v>43749</v>
       </c>
@@ -8145,7 +8586,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A19" s="59">
         <v>43750</v>
       </c>
@@ -8168,7 +8609,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="59">
         <v>43751</v>
       </c>
@@ -8191,7 +8632,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="59">
         <v>43751</v>
       </c>
@@ -8214,7 +8655,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="59">
         <v>43753</v>
       </c>
@@ -8237,7 +8678,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -8246,7 +8687,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -8255,7 +8696,7 @@
       <c r="F24" s="17"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -8264,7 +8705,7 @@
       <c r="F25" s="17"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -8273,7 +8714,7 @@
       <c r="F26" s="17"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -8282,7 +8723,7 @@
       <c r="F27" s="17"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -8291,7 +8732,7 @@
       <c r="F28" s="17"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -8300,7 +8741,7 @@
       <c r="F29" s="17"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -8309,7 +8750,7 @@
       <c r="F30" s="17"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -8318,7 +8759,7 @@
       <c r="F31" s="17"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -8327,7 +8768,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -8336,7 +8777,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -8345,7 +8786,7 @@
       <c r="F34" s="17"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -8354,7 +8795,7 @@
       <c r="F35" s="17"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -8363,7 +8804,7 @@
       <c r="F36" s="9"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -8372,7 +8813,7 @@
       <c r="F37" s="9"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -8398,20 +8839,20 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="46.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="46.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
@@ -8424,10 +8865,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
     </row>
-    <row r="3" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>39</v>
       </c>
@@ -8438,8 +8879,8 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:7" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:7" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>32</v>
       </c>
@@ -8462,7 +8903,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>55</v>
       </c>
@@ -8485,7 +8926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>55</v>
       </c>
@@ -8508,7 +8949,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>42</v>
       </c>
@@ -8531,7 +8972,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>50</v>
       </c>
@@ -8554,7 +8995,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>45</v>
       </c>
@@ -8577,7 +9018,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -8586,7 +9027,7 @@
       <c r="F11" s="18"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -8595,7 +9036,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -8604,7 +9045,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -8613,7 +9054,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -8622,7 +9063,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -8631,7 +9072,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -8640,7 +9081,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -8649,7 +9090,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="19"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -8658,7 +9099,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -8667,7 +9108,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -8676,7 +9117,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -8685,7 +9126,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -8694,7 +9135,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -8703,7 +9144,7 @@
       <c r="F24" s="17"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -8712,7 +9153,7 @@
       <c r="F25" s="17"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -8721,7 +9162,7 @@
       <c r="F26" s="17"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -8730,7 +9171,7 @@
       <c r="F27" s="17"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -8739,7 +9180,7 @@
       <c r="F28" s="17"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -8748,7 +9189,7 @@
       <c r="F29" s="17"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -8757,7 +9198,7 @@
       <c r="F30" s="17"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -8766,7 +9207,7 @@
       <c r="F31" s="17"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -8775,7 +9216,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -8784,7 +9225,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -8793,7 +9234,7 @@
       <c r="F34" s="17"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -8802,7 +9243,7 @@
       <c r="F35" s="17"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -8811,7 +9252,7 @@
       <c r="F36" s="9"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -8820,7 +9261,7 @@
       <c r="F37" s="9"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -8845,21 +9286,21 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="125" workbookViewId="0">
+    <sheetView zoomScaleNormal="125" workbookViewId="0">
       <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="46.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="46.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
@@ -8872,10 +9313,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
     </row>
-    <row r="3" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>39</v>
       </c>
@@ -8886,8 +9327,8 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:7" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:7" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>32</v>
       </c>
@@ -8910,7 +9351,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>43715</v>
       </c>
@@ -8933,7 +9374,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>43727</v>
       </c>
@@ -8956,7 +9397,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>43727</v>
       </c>
@@ -8979,7 +9420,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>43728</v>
       </c>
@@ -9002,7 +9443,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A10" s="46">
         <v>43735</v>
       </c>
@@ -9025,7 +9466,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="46">
         <v>43737</v>
       </c>
@@ -9048,7 +9489,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="46">
         <v>43738</v>
       </c>
@@ -9071,7 +9512,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A13" s="46">
         <v>43739</v>
       </c>
@@ -9094,7 +9535,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A14" s="39">
         <v>43739</v>
       </c>
@@ -9117,7 +9558,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A15" s="46">
         <v>43744</v>
       </c>
@@ -9140,7 +9581,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A16" s="46">
         <v>43744</v>
       </c>
@@ -9163,7 +9604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A17" s="46">
         <v>43744</v>
       </c>
@@ -9186,7 +9627,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="59">
         <v>43749</v>
       </c>
@@ -9209,7 +9650,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="59">
         <v>43751</v>
       </c>
@@ -9232,7 +9673,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A20" s="59">
         <v>43751</v>
       </c>
@@ -9255,7 +9696,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="59">
         <v>43752</v>
       </c>
@@ -9278,7 +9719,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="59">
         <v>43752</v>
       </c>
@@ -9301,7 +9742,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A23" s="59">
         <v>43753</v>
       </c>
@@ -9324,7 +9765,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="67">
         <v>43753</v>
       </c>
@@ -9347,7 +9788,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A25" s="67">
         <v>43754</v>
       </c>
@@ -9370,7 +9811,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="67">
         <v>43754</v>
       </c>
@@ -9393,7 +9834,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="67">
         <v>43755</v>
       </c>
@@ -9416,7 +9857,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="67">
         <v>43755</v>
       </c>
@@ -9439,7 +9880,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="67">
         <v>43755</v>
       </c>
@@ -9462,7 +9903,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14">
         <v>43760</v>
       </c>
@@ -9485,7 +9926,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14">
         <v>43762</v>
       </c>
@@ -9508,7 +9949,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -9517,7 +9958,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -9526,7 +9967,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -9535,7 +9976,7 @@
       <c r="F34" s="17"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -9544,7 +9985,7 @@
       <c r="F35" s="17"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -9553,7 +9994,7 @@
       <c r="F36" s="9"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -9562,7 +10003,7 @@
       <c r="F37" s="9"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -9588,20 +10029,20 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="46.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="46.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
@@ -9614,10 +10055,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
     </row>
-    <row r="3" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>39</v>
       </c>
@@ -9628,8 +10069,8 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:7" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:7" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>32</v>
       </c>
@@ -9652,7 +10093,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>44</v>
       </c>
@@ -9675,7 +10116,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>55</v>
       </c>
@@ -9698,7 +10139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>55</v>
       </c>
@@ -9721,7 +10162,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>42</v>
       </c>
@@ -9744,7 +10185,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
@@ -9767,7 +10208,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>30</v>
       </c>
@@ -9790,7 +10231,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>53</v>
       </c>
@@ -9813,7 +10254,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>34</v>
       </c>
@@ -9836,7 +10277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>33</v>
       </c>
@@ -9859,7 +10300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>81</v>
       </c>
@@ -9882,7 +10323,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>82</v>
       </c>
@@ -9905,7 +10346,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -9914,7 +10355,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -9923,7 +10364,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="19"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -9932,7 +10373,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -9941,7 +10382,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -9950,7 +10391,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -9959,7 +10400,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -9968,7 +10409,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -9977,7 +10418,7 @@
       <c r="F24" s="17"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -9986,7 +10427,7 @@
       <c r="F25" s="17"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -9995,7 +10436,7 @@
       <c r="F26" s="17"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -10004,7 +10445,7 @@
       <c r="F27" s="17"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -10013,7 +10454,7 @@
       <c r="F28" s="17"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -10022,7 +10463,7 @@
       <c r="F29" s="17"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -10031,7 +10472,7 @@
       <c r="F30" s="17"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -10040,7 +10481,7 @@
       <c r="F31" s="17"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -10049,7 +10490,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -10058,7 +10499,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -10067,7 +10508,7 @@
       <c r="F34" s="17"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -10076,7 +10517,7 @@
       <c r="F35" s="17"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -10085,7 +10526,7 @@
       <c r="F36" s="9"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -10094,7 +10535,7 @@
       <c r="F37" s="9"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -10123,17 +10564,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="8" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="46.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="46.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
@@ -10146,10 +10587,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
     </row>
-    <row r="3" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>39</v>
       </c>
@@ -10160,8 +10601,8 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:7" s="11" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="11.85" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:7" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>32</v>
       </c>
@@ -10184,7 +10625,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -10193,7 +10634,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="19"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -10202,7 +10643,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -10211,7 +10652,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -10220,7 +10661,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -10229,7 +10670,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -10238,7 +10679,7 @@
       <c r="F11" s="18"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -10247,7 +10688,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -10256,7 +10697,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -10265,7 +10706,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -10274,7 +10715,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -10283,7 +10724,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -10292,7 +10733,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -10301,7 +10742,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="19"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -10310,7 +10751,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -10319,7 +10760,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -10328,7 +10769,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="19"/>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -10337,7 +10778,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -10346,7 +10787,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -10355,7 +10796,7 @@
       <c r="F24" s="17"/>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -10364,7 +10805,7 @@
       <c r="F25" s="17"/>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -10373,7 +10814,7 @@
       <c r="F26" s="17"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -10382,7 +10823,7 @@
       <c r="F27" s="17"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="14"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -10391,7 +10832,7 @@
       <c r="F28" s="17"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -10400,7 +10841,7 @@
       <c r="F29" s="17"/>
       <c r="G29" s="4"/>
     </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -10409,7 +10850,7 @@
       <c r="F30" s="17"/>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -10418,7 +10859,7 @@
       <c r="F31" s="17"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -10427,7 +10868,7 @@
       <c r="F32" s="17"/>
       <c r="G32" s="4"/>
     </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -10436,7 +10877,7 @@
       <c r="F33" s="17"/>
       <c r="G33" s="4"/>
     </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -10445,7 +10886,7 @@
       <c r="F34" s="17"/>
       <c r="G34" s="4"/>
     </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -10454,7 +10895,7 @@
       <c r="F35" s="17"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -10463,7 +10904,7 @@
       <c r="F36" s="9"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -10472,7 +10913,7 @@
       <c r="F37" s="9"/>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>

</xml_diff>